<commit_message>
Removal of jupyter notebook files and corrections
</commit_message>
<xml_diff>
--- a/frame/m_matrix.xlsx
+++ b/frame/m_matrix.xlsx
@@ -412,7 +412,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>781714285.7142857</v>
+        <v>771797499.4876</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -430,13 +430,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -453,19 +453,19 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>2408956268.221574</v>
+        <v>2408631579.893814</v>
       </c>
       <c r="C3">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-8956268.221574347</v>
+        <v>-8631579.893813588</v>
       </c>
       <c r="F3">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -491,28 +491,28 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
       <c r="C4">
-        <v>164571428.5714286</v>
+        <v>153660284.3409755</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
       <c r="F4">
-        <v>18285714.28571429</v>
+        <v>17291356.28194697</v>
       </c>
       <c r="G4">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>32000000.00000001</v>
+        <v>27041606.88665711</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>781714285.7142857</v>
+        <v>771797499.4876</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -553,13 +553,13 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -567,19 +567,19 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>-8956268.221574347</v>
+        <v>-8631579.893813588</v>
       </c>
       <c r="C6">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2408956268.221574</v>
+        <v>2408631579.893814</v>
       </c>
       <c r="F6">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -605,19 +605,19 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
       <c r="C7">
-        <v>18285714.28571429</v>
+        <v>17291356.28194697</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
       <c r="F7">
-        <v>164571428.5714286</v>
+        <v>153660284.3409755</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -629,24 +629,24 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>32000000.00000001</v>
+        <v>27041606.88665711</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -658,13 +658,13 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>733714285.7142857</v>
+        <v>728755892.6009429</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
       <c r="J8">
         <v>-685714285.7142857</v>
@@ -699,30 +699,30 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1208956268.221574</v>
+        <v>1208631579.893814</v>
       </c>
       <c r="I9">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>-8956268.221574347</v>
+        <v>-8631579.893813588</v>
       </c>
       <c r="L9">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>32000000.00000001</v>
+        <v>27041606.88665711</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -734,22 +734,22 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
       <c r="H10">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
       <c r="I10">
-        <v>100571428.5714286</v>
+        <v>94618677.45431837</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
       <c r="L10">
-        <v>18285714.28571429</v>
+        <v>17291356.28194697</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -763,13 +763,13 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
       <c r="G11">
         <v>-685714285.7142857</v>
@@ -781,13 +781,13 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>733714285.7142857</v>
+        <v>728755892.6009429</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -813,19 +813,19 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>-8956268.221574347</v>
+        <v>-8631579.893813588</v>
       </c>
       <c r="I12">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
-        <v>1208956268.221574</v>
+        <v>1208631579.893814</v>
       </c>
       <c r="L12">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -839,31 +839,31 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>-48000000.00000001</v>
+        <v>-43041606.88665712</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>32000000.00000001</v>
+        <v>27041606.88665711</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>15673469.38775511</v>
+        <v>15105264.81417378</v>
       </c>
       <c r="I13">
-        <v>18285714.28571429</v>
+        <v>17291356.28194697</v>
       </c>
       <c r="J13">
-        <v>48000000.00000001</v>
+        <v>43041606.88665712</v>
       </c>
       <c r="K13">
-        <v>-15673469.38775511</v>
+        <v>-15105264.81417378</v>
       </c>
       <c r="L13">
-        <v>100571428.5714286</v>
+        <v>94618677.45431837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>